<commit_message>
lo he runeado otra vez xd
</commit_message>
<xml_diff>
--- a/M7/final/Results.xlsx
+++ b/M7/final/Results.xlsx
@@ -456,10 +456,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>523</v>
+        <v>518</v>
       </c>
     </row>
     <row r="3">
@@ -467,10 +467,10 @@
         <v>0</v>
       </c>
       <c r="B3" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="4">
@@ -478,10 +478,10 @@
         <v>0</v>
       </c>
       <c r="B4" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C4" t="n">
-        <v>458</v>
+        <v>579</v>
       </c>
     </row>
     <row r="5">
@@ -489,10 +489,10 @@
         <v>0</v>
       </c>
       <c r="B5" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C5" t="n">
-        <v>258</v>
+        <v>136</v>
       </c>
     </row>
     <row r="6">
@@ -500,10 +500,10 @@
         <v>0</v>
       </c>
       <c r="B6" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C6" t="n">
-        <v>521</v>
+        <v>458</v>
       </c>
     </row>
     <row r="7">
@@ -511,10 +511,10 @@
         <v>0</v>
       </c>
       <c r="B7" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C7" t="n">
-        <v>199</v>
+        <v>256</v>
       </c>
     </row>
     <row r="8">
@@ -522,10 +522,10 @@
         <v>0</v>
       </c>
       <c r="B8" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C8" t="n">
-        <v>638</v>
+        <v>459</v>
       </c>
     </row>
     <row r="9">
@@ -533,10 +533,10 @@
         <v>0</v>
       </c>
       <c r="B9" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C9" t="n">
-        <v>76</v>
+        <v>256</v>
       </c>
     </row>
     <row r="10">
@@ -544,10 +544,10 @@
         <v>0</v>
       </c>
       <c r="B10" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C10" t="n">
-        <v>572</v>
+        <v>457</v>
       </c>
     </row>
     <row r="11">
@@ -555,10 +555,10 @@
         <v>0</v>
       </c>
       <c r="B11" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C11" t="n">
-        <v>248</v>
+        <v>260</v>
       </c>
     </row>
     <row r="12">
@@ -566,10 +566,10 @@
         <v>0</v>
       </c>
       <c r="B12" t="n">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C12" t="n">
-        <v>133</v>
+        <v>578</v>
       </c>
     </row>
     <row r="13">
@@ -577,10 +577,10 @@
         <v>0</v>
       </c>
       <c r="B13" t="n">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C13" t="n">
-        <v>262</v>
+        <v>135</v>
       </c>
     </row>
     <row r="14">
@@ -588,10 +588,10 @@
         <v>0</v>
       </c>
       <c r="B14" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C14" t="n">
-        <v>141</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15">
@@ -599,10 +599,10 @@
         <v>0</v>
       </c>
       <c r="B15" t="n">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C15" t="n">
-        <v>576</v>
+        <v>323</v>
       </c>
     </row>
     <row r="16">
@@ -610,10 +610,10 @@
         <v>0</v>
       </c>
       <c r="B16" t="n">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C16" t="n">
-        <v>190</v>
+        <v>265</v>
       </c>
     </row>
     <row r="17">
@@ -621,10 +621,10 @@
         <v>0</v>
       </c>
       <c r="B17" t="n">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="C17" t="n">
-        <v>11</v>
+        <v>395</v>
       </c>
     </row>
     <row r="18">
@@ -632,10 +632,10 @@
         <v>0</v>
       </c>
       <c r="B18" t="n">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="C18" t="n">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="19">
@@ -643,10 +643,10 @@
         <v>0</v>
       </c>
       <c r="B19" t="n">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="C19" t="n">
-        <v>259</v>
+        <v>449</v>
       </c>
     </row>
     <row r="20">
@@ -654,10 +654,10 @@
         <v>0</v>
       </c>
       <c r="B20" t="n">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="C20" t="n">
-        <v>640</v>
+        <v>259</v>
       </c>
     </row>
     <row r="21">
@@ -665,186 +665,186 @@
         <v>0</v>
       </c>
       <c r="B21" t="n">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="C21" t="n">
-        <v>75</v>
+        <v>926</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B22" t="n">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C22" t="n">
-        <v>128</v>
+        <v>916</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B23" t="n">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="C23" t="n">
-        <v>315</v>
+        <v>131</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B24" t="n">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="C24" t="n">
-        <v>142</v>
+        <v>520</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B25" t="n">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="C25" t="n">
-        <v>459</v>
+        <v>77</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B26" t="n">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="C26" t="n">
-        <v>255</v>
+        <v>522</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C27" t="n">
-        <v>928</v>
+        <v>15</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B28" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="C28" t="n">
-        <v>928</v>
+        <v>584</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B29" t="n">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C29" t="n">
-        <v>511</v>
+        <v>4</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B30" t="n">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C30" t="n">
-        <v>255</v>
+        <v>643</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B31" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C31" t="n">
-        <v>508</v>
+        <v>4</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B32" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C32" t="n">
-        <v>312</v>
+        <v>644</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B33" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C33" t="n">
-        <v>927</v>
+        <v>264</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B34" t="n">
         <v>8</v>
       </c>
       <c r="C34" t="n">
-        <v>927</v>
+        <v>265</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B35" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C35" t="n">
-        <v>927</v>
+        <v>699</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B36" t="n">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="C36" t="n">
-        <v>927</v>
+        <v>697</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B37" t="n">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C37" t="n">
-        <v>927</v>
+        <v>646</v>
       </c>
     </row>
   </sheetData>
@@ -923,7 +923,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C2" t="n">
         <v>179.8055404066405</v>
@@ -935,10 +935,10 @@
         <v>8.40570843560528</v>
       </c>
       <c r="F2" t="n">
-        <v>0.1912045889101338</v>
+        <v>0.1930501930501931</v>
       </c>
       <c r="G2" t="n">
-        <v>19120.45889101338</v>
+        <v>19305.0193050193</v>
       </c>
       <c r="H2" t="n">
         <v>179.8055404066405</v>
@@ -955,7 +955,7 @@
         <v>0</v>
       </c>
       <c r="B3" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C3" t="n">
         <v>179.8055404066405</v>
@@ -967,10 +967,10 @@
         <v>8.40570843560528</v>
       </c>
       <c r="F3" t="n">
-        <v>0.2183406113537118</v>
+        <v>0.1727115716753022</v>
       </c>
       <c r="G3" t="n">
-        <v>21834.06113537118</v>
+        <v>17271.15716753023</v>
       </c>
       <c r="H3" t="n">
         <v>179.8055404066405</v>
@@ -987,7 +987,7 @@
         <v>0</v>
       </c>
       <c r="B4" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C4" t="n">
         <v>179.8055404066405</v>
@@ -999,10 +999,10 @@
         <v>8.40570843560528</v>
       </c>
       <c r="F4" t="n">
-        <v>0.1919385796545106</v>
+        <v>0.2183406113537118</v>
       </c>
       <c r="G4" t="n">
-        <v>19193.85796545105</v>
+        <v>21834.06113537118</v>
       </c>
       <c r="H4" t="n">
         <v>179.8055404066405</v>
@@ -1019,7 +1019,7 @@
         <v>0</v>
       </c>
       <c r="B5" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5" t="n">
         <v>179.8055404066405</v>
@@ -1031,10 +1031,10 @@
         <v>8.40570843560528</v>
       </c>
       <c r="F5" t="n">
-        <v>0.1567398119122257</v>
+        <v>0.2178649237472767</v>
       </c>
       <c r="G5" t="n">
-        <v>15673.98119122257</v>
+        <v>21786.49237472767</v>
       </c>
       <c r="H5" t="n">
         <v>179.8055404066405</v>
@@ -1051,7 +1051,7 @@
         <v>0</v>
       </c>
       <c r="B6" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C6" t="n">
         <v>179.8055404066405</v>
@@ -1063,10 +1063,10 @@
         <v>8.40570843560528</v>
       </c>
       <c r="F6" t="n">
-        <v>0.1748251748251748</v>
+        <v>0.2188183807439825</v>
       </c>
       <c r="G6" t="n">
-        <v>17482.51748251748</v>
+        <v>21881.83807439825</v>
       </c>
       <c r="H6" t="n">
         <v>179.8055404066405</v>
@@ -1083,7 +1083,7 @@
         <v>0</v>
       </c>
       <c r="B7" t="n">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C7" t="n">
         <v>179.8055404066405</v>
@@ -1095,10 +1095,10 @@
         <v>8.40570843560528</v>
       </c>
       <c r="F7" t="n">
-        <v>0.7518796992481203</v>
+        <v>0.1730103806228374</v>
       </c>
       <c r="G7" t="n">
-        <v>75187.96992481203</v>
+        <v>17301.03806228374</v>
       </c>
       <c r="H7" t="n">
         <v>179.8055404066405</v>
@@ -1115,7 +1115,7 @@
         <v>0</v>
       </c>
       <c r="B8" t="n">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C8" t="n">
         <v>179.8055404066405</v>
@@ -1127,10 +1127,10 @@
         <v>8.40570843560528</v>
       </c>
       <c r="F8" t="n">
-        <v>0.1736111111111111</v>
+        <v>9.090909090909092</v>
       </c>
       <c r="G8" t="n">
-        <v>17361.11111111111</v>
+        <v>909090.9090909091</v>
       </c>
       <c r="H8" t="n">
         <v>179.8055404066405</v>
@@ -1147,7 +1147,7 @@
         <v>0</v>
       </c>
       <c r="B9" t="n">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="C9" t="n">
         <v>179.8055404066405</v>
@@ -1159,10 +1159,10 @@
         <v>8.40570843560528</v>
       </c>
       <c r="F9" t="n">
-        <v>9.090909090909092</v>
+        <v>0.2531645569620253</v>
       </c>
       <c r="G9" t="n">
-        <v>909090.9090909091</v>
+        <v>25316.45569620253</v>
       </c>
       <c r="H9" t="n">
         <v>179.8055404066405</v>
@@ -1179,7 +1179,7 @@
         <v>0</v>
       </c>
       <c r="B10" t="n">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="C10" t="n">
         <v>179.8055404066405</v>
@@ -1191,10 +1191,10 @@
         <v>8.40570843560528</v>
       </c>
       <c r="F10" t="n">
-        <v>0.15625</v>
+        <v>0.22271714922049</v>
       </c>
       <c r="G10" t="n">
-        <v>15625</v>
+        <v>22271.714922049</v>
       </c>
       <c r="H10" t="n">
         <v>179.8055404066405</v>
@@ -1211,7 +1211,7 @@
         <v>0</v>
       </c>
       <c r="B11" t="n">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C11" t="n">
         <v>179.8055404066405</v>
@@ -1223,10 +1223,10 @@
         <v>8.40570843560528</v>
       </c>
       <c r="F11" t="n">
-        <v>0.78125</v>
+        <v>0.1079913606911447</v>
       </c>
       <c r="G11" t="n">
-        <v>78125</v>
+        <v>10799.13606911447</v>
       </c>
       <c r="H11" t="n">
         <v>179.8055404066405</v>
@@ -1240,10 +1240,10 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B12" t="n">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="C12" t="n">
         <v>179.8055404066405</v>
@@ -1255,10 +1255,10 @@
         <v>8.40570843560528</v>
       </c>
       <c r="F12" t="n">
-        <v>0.2178649237472767</v>
+        <v>0.1091703056768559</v>
       </c>
       <c r="G12" t="n">
-        <v>21786.49237472767</v>
+        <v>10917.03056768559</v>
       </c>
       <c r="H12" t="n">
         <v>179.8055404066405</v>
@@ -1272,10 +1272,10 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B13" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C13" t="n">
         <v>179.8055404066405</v>
@@ -1287,10 +1287,10 @@
         <v>8.40570843560528</v>
       </c>
       <c r="F13" t="n">
-        <v>0.1077586206896552</v>
+        <v>0.7633587786259542</v>
       </c>
       <c r="G13" t="n">
-        <v>10775.86206896552</v>
+        <v>76335.87786259541</v>
       </c>
       <c r="H13" t="n">
         <v>179.8055404066405</v>
@@ -1304,10 +1304,10 @@
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B14" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C14" t="n">
         <v>179.8055404066405</v>
@@ -1319,10 +1319,10 @@
         <v>8.40570843560528</v>
       </c>
       <c r="F14" t="n">
-        <v>0.1077586206896552</v>
+        <v>1.298701298701299</v>
       </c>
       <c r="G14" t="n">
-        <v>10775.86206896552</v>
+        <v>129870.1298701299</v>
       </c>
       <c r="H14" t="n">
         <v>179.8055404066405</v>
@@ -1336,10 +1336,10 @@
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B15" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="C15" t="n">
         <v>179.8055404066405</v>
@@ -1351,10 +1351,10 @@
         <v>8.40570843560528</v>
       </c>
       <c r="F15" t="n">
-        <v>0.1956947162426614</v>
+        <v>6.666666666666667</v>
       </c>
       <c r="G15" t="n">
-        <v>19569.47162426615</v>
+        <v>666666.6666666666</v>
       </c>
       <c r="H15" t="n">
         <v>179.8055404066405</v>
@@ -1368,10 +1368,10 @@
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B16" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C16" t="n">
         <v>179.8055404066405</v>
@@ -1383,10 +1383,10 @@
         <v>8.40570843560528</v>
       </c>
       <c r="F16" t="n">
-        <v>0.1968503937007874</v>
+        <v>25</v>
       </c>
       <c r="G16" t="n">
-        <v>19685.03937007874</v>
+        <v>2500000</v>
       </c>
       <c r="H16" t="n">
         <v>179.8055404066405</v>
@@ -1400,10 +1400,10 @@
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B17" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C17" t="n">
         <v>179.8055404066405</v>
@@ -1415,10 +1415,10 @@
         <v>8.40570843560528</v>
       </c>
       <c r="F17" t="n">
-        <v>0.1078748651564186</v>
+        <v>25</v>
       </c>
       <c r="G17" t="n">
-        <v>10787.48651564185</v>
+        <v>2500000</v>
       </c>
       <c r="H17" t="n">
         <v>179.8055404066405</v>
@@ -1432,7 +1432,7 @@
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B18" t="n">
         <v>8</v>
@@ -1447,10 +1447,10 @@
         <v>8.40570843560528</v>
       </c>
       <c r="F18" t="n">
-        <v>0.1078748651564186</v>
+        <v>0.3787878787878788</v>
       </c>
       <c r="G18" t="n">
-        <v>10787.48651564185</v>
+        <v>37878.78787878788</v>
       </c>
       <c r="H18" t="n">
         <v>179.8055404066405</v>
@@ -1464,10 +1464,10 @@
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B19" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C19" t="n">
         <v>179.8055404066405</v>
@@ -1479,10 +1479,10 @@
         <v>8.40570843560528</v>
       </c>
       <c r="F19" t="n">
-        <v>0.1078748651564186</v>
+        <v>0.1430615164520744</v>
       </c>
       <c r="G19" t="n">
-        <v>10787.48651564185</v>
+        <v>14306.15164520744</v>
       </c>
       <c r="H19" t="n">
         <v>179.8055404066405</v>
@@ -1496,10 +1496,10 @@
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B20" t="n">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="C20" t="n">
         <v>179.8055404066405</v>
@@ -1511,10 +1511,10 @@
         <v>8.40570843560528</v>
       </c>
       <c r="F20" t="n">
-        <v>0.1078748651564186</v>
+        <v>0.1434720229555237</v>
       </c>
       <c r="G20" t="n">
-        <v>10787.48651564185</v>
+        <v>14347.20229555237</v>
       </c>
       <c r="H20" t="n">
         <v>179.8055404066405</v>
@@ -1528,10 +1528,10 @@
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B21" t="n">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C21" t="n">
         <v>179.8055404066405</v>
@@ -1543,10 +1543,10 @@
         <v>8.40570843560528</v>
       </c>
       <c r="F21" t="n">
-        <v>0.1078748651564186</v>
+        <v>0.1547987616099071</v>
       </c>
       <c r="G21" t="n">
-        <v>10787.48651564185</v>
+        <v>15479.87616099071</v>
       </c>
       <c r="H21" t="n">
         <v>179.8055404066405</v>

</xml_diff>